<commit_message>
Price change model optimization.
</commit_message>
<xml_diff>
--- a/Data/raw_stock_data.xlsx
+++ b/Data/raw_stock_data.xlsx
@@ -2,46 +2,36 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\NTUT\Other\113IFM_camp\IFM_camp_bot\Bot\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/770c45f6cc28d03d/桌面/資財營/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F8F17F-40D0-45CD-B174-7E07ED946401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F7F8F17F-40D0-45CD-B174-7E07ED946401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80454AF0-3F88-429E-B7B7-328AFE7067D6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F8FD49BE-BC86-4C92-8F4D-99B84D176403}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F8FD49BE-BC86-4C92-8F4D-99B84D176403}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="2" r:id="rId1"/>
-    <sheet name="initial_data" sheetId="3" r:id="rId2"/>
-    <sheet name="Q4" sheetId="1" r:id="rId3"/>
-    <sheet name="Q1" sheetId="4" r:id="rId4"/>
-    <sheet name="Q2" sheetId="5" r:id="rId5"/>
-    <sheet name="Q3" sheetId="6" r:id="rId6"/>
+    <sheet name="price_change" sheetId="7" r:id="rId2"/>
+    <sheet name="initial_data" sheetId="3" r:id="rId3"/>
+    <sheet name="Q4" sheetId="1" r:id="rId4"/>
+    <sheet name="Q1" sheetId="4" r:id="rId5"/>
+    <sheet name="Q2" sheetId="5" r:id="rId6"/>
+    <sheet name="Q3" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="51">
   <si>
     <t>base_period_eps</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -189,6 +179,42 @@
   </si>
   <si>
     <t>sector</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>每輪秒數</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>變動頻率</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>變動次數</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>close</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R4</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -301,7 +327,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -379,6 +405,15 @@
     </xf>
     <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -717,47 +752,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5B1930-18B5-46DE-91AC-AB66E4E6FDB4}">
   <dimension ref="A1:AI12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE3" sqref="AE3:AE12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="12.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.08984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.25" style="2" customWidth="1"/>
-    <col min="17" max="17" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.6328125" style="2" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="28.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="36" max="16384" width="9" style="2"/>
   </cols>
@@ -914,7 +949,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="15.75">
+    <row r="3" spans="1:35" ht="15.5">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -945,6 +980,7 @@
         <v>0.125</v>
       </c>
       <c r="J3" s="13">
+        <f>price_change!D3</f>
         <v>1</v>
       </c>
       <c r="K3" s="12">
@@ -968,6 +1004,7 @@
         <v>0.16669999999999999</v>
       </c>
       <c r="Q3" s="13">
+        <f>price_change!H3</f>
         <v>1</v>
       </c>
       <c r="R3" s="12">
@@ -991,6 +1028,7 @@
         <v>-0.47620000000000001</v>
       </c>
       <c r="X3" s="13">
+        <f>price_change!L3</f>
         <v>1</v>
       </c>
       <c r="Y3" s="12">
@@ -1014,7 +1052,8 @@
         <v>1</v>
       </c>
       <c r="AE3" s="13">
-        <v>1</v>
+        <f>price_change!P3</f>
+        <v>0.8</v>
       </c>
       <c r="AF3" s="12">
         <v>9800000</v>
@@ -1029,7 +1068,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="15.75">
+    <row r="4" spans="1:35" ht="15.5">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1060,6 +1099,7 @@
         <v>7.1400000000000005E-2</v>
       </c>
       <c r="J4" s="13">
+        <f>price_change!D4</f>
         <v>1</v>
       </c>
       <c r="K4" s="12">
@@ -1083,6 +1123,7 @@
         <v>0.2</v>
       </c>
       <c r="Q4" s="13">
+        <f>price_change!H4</f>
         <v>1</v>
       </c>
       <c r="R4" s="12">
@@ -1106,6 +1147,7 @@
         <v>-8.3299999999999999E-2</v>
       </c>
       <c r="X4" s="13">
+        <f>price_change!L4</f>
         <v>1</v>
       </c>
       <c r="Y4" s="12">
@@ -1129,7 +1171,8 @@
         <v>0.39389999999999997</v>
       </c>
       <c r="AE4" s="13">
-        <v>1</v>
+        <f>price_change!P4</f>
+        <v>0.9</v>
       </c>
       <c r="AF4" s="12">
         <v>4800000</v>
@@ -1144,7 +1187,7 @@
         <v>2300000</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15.75">
+    <row r="5" spans="1:35" ht="15.5">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1175,6 +1218,7 @@
         <v>0.1</v>
       </c>
       <c r="J5" s="13">
+        <f>price_change!D5</f>
         <v>1</v>
       </c>
       <c r="K5" s="12">
@@ -1198,7 +1242,8 @@
         <v>-1.0909</v>
       </c>
       <c r="Q5" s="13">
-        <v>1</v>
+        <f>price_change!H5</f>
+        <v>0.2</v>
       </c>
       <c r="R5" s="12">
         <v>2500000</v>
@@ -1221,7 +1266,8 @@
         <v>-3</v>
       </c>
       <c r="X5" s="13">
-        <v>1</v>
+        <f>price_change!L5</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="Y5" s="12">
         <v>2000000</v>
@@ -1244,7 +1290,8 @@
         <v>6</v>
       </c>
       <c r="AE5" s="13">
-        <v>1</v>
+        <f>price_change!P5</f>
+        <v>0.15</v>
       </c>
       <c r="AF5" s="12">
         <v>5000000</v>
@@ -1259,7 +1306,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="15.75">
+    <row r="6" spans="1:35" ht="15.5">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1290,6 +1337,7 @@
         <v>7.1400000000000005E-2</v>
       </c>
       <c r="J6" s="13">
+        <f>price_change!D6</f>
         <v>1</v>
       </c>
       <c r="K6" s="12">
@@ -1313,6 +1361,7 @@
         <v>0.31669999999999998</v>
       </c>
       <c r="Q6" s="13">
+        <f>price_change!H6</f>
         <v>1</v>
       </c>
       <c r="R6" s="12">
@@ -1336,7 +1385,8 @@
         <v>-0.50629999999999997</v>
       </c>
       <c r="X6" s="13">
-        <v>1</v>
+        <f>price_change!L6</f>
+        <v>0.7</v>
       </c>
       <c r="Y6" s="12">
         <v>7900000</v>
@@ -1359,7 +1409,8 @@
         <v>1.1026</v>
       </c>
       <c r="AE6" s="13">
-        <v>1</v>
+        <f>price_change!P6</f>
+        <v>0.8</v>
       </c>
       <c r="AF6" s="12">
         <v>8800000</v>
@@ -1374,7 +1425,7 @@
         <v>4100000</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="15.75">
+    <row r="7" spans="1:35" ht="15.5">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1405,7 +1456,8 @@
         <v>-0.1211</v>
       </c>
       <c r="J7" s="13">
-        <v>1</v>
+        <f>price_change!D7</f>
+        <v>0.4</v>
       </c>
       <c r="K7" s="12">
         <v>600000</v>
@@ -1428,7 +1480,8 @@
         <v>-9.0300000000000005E-2</v>
       </c>
       <c r="Q7" s="13">
-        <v>1</v>
+        <f>price_change!H7</f>
+        <v>0.3</v>
       </c>
       <c r="R7" s="12">
         <v>450000</v>
@@ -1451,7 +1504,8 @@
         <v>-1.7899999999999999E-2</v>
       </c>
       <c r="X7" s="13">
-        <v>1</v>
+        <f>price_change!L7</f>
+        <v>0.8</v>
       </c>
       <c r="Y7" s="12">
         <v>446000</v>
@@ -1474,6 +1528,7 @@
         <v>9.0899999999999995E-2</v>
       </c>
       <c r="AE7" s="13">
+        <f>price_change!P7</f>
         <v>1</v>
       </c>
       <c r="AF7" s="12">
@@ -1489,7 +1544,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="15.75">
+    <row r="8" spans="1:35" ht="15.5">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1520,6 +1575,7 @@
         <v>5.8799999999999998E-2</v>
       </c>
       <c r="J8" s="13">
+        <f>price_change!D8</f>
         <v>1</v>
       </c>
       <c r="K8" s="12">
@@ -1543,7 +1599,8 @@
         <v>0.77410000000000001</v>
       </c>
       <c r="Q8" s="13">
-        <v>1</v>
+        <f>price_change!H8</f>
+        <v>0.7</v>
       </c>
       <c r="R8" s="12">
         <v>650000</v>
@@ -1566,7 +1623,8 @@
         <v>-0.16489999999999999</v>
       </c>
       <c r="X8" s="13">
-        <v>1</v>
+        <f>price_change!L8</f>
+        <v>0.65</v>
       </c>
       <c r="Y8" s="12">
         <v>620000</v>
@@ -1589,6 +1647,7 @@
         <v>-1.2500000000000001E-2</v>
       </c>
       <c r="AE8" s="13">
+        <f>price_change!P8</f>
         <v>1</v>
       </c>
       <c r="AF8" s="12">
@@ -1604,7 +1663,7 @@
         <v>395000</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="15.75">
+    <row r="9" spans="1:35" ht="15.5">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1635,7 +1694,8 @@
         <v>-0.1237</v>
       </c>
       <c r="J9" s="13">
-        <v>1</v>
+        <f>price_change!D9</f>
+        <v>0.45</v>
       </c>
       <c r="K9" s="12">
         <v>700000</v>
@@ -1658,7 +1718,8 @@
         <v>0.45590000000000003</v>
       </c>
       <c r="Q9" s="13">
-        <v>1</v>
+        <f>price_change!H9</f>
+        <v>0.5</v>
       </c>
       <c r="R9" s="12">
         <v>1100000</v>
@@ -1681,6 +1742,7 @@
         <v>0.1414</v>
       </c>
       <c r="X9" s="13">
+        <f>price_change!L9</f>
         <v>1</v>
       </c>
       <c r="Y9" s="12">
@@ -1704,6 +1766,7 @@
         <v>0.1381</v>
       </c>
       <c r="AE9" s="13">
+        <f>price_change!P9</f>
         <v>1</v>
       </c>
       <c r="AF9" s="12">
@@ -1719,7 +1782,7 @@
         <v>643000</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="15.75">
+    <row r="10" spans="1:35" ht="15.5">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1750,6 +1813,7 @@
         <v>3.4500000000000003E-2</v>
       </c>
       <c r="J10" s="13">
+        <f>price_change!D10</f>
         <v>1</v>
       </c>
       <c r="K10" s="12">
@@ -1773,7 +1837,8 @@
         <v>-1.0432999999999999</v>
       </c>
       <c r="Q10" s="13">
-        <v>1</v>
+        <f>price_change!H10</f>
+        <v>0.05</v>
       </c>
       <c r="R10" s="12">
         <v>470610</v>
@@ -1796,7 +1861,8 @@
         <v>12.538500000000001</v>
       </c>
       <c r="X10" s="13">
-        <v>1</v>
+        <f>price_change!L10</f>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="Y10" s="12">
         <v>870610</v>
@@ -1819,7 +1885,8 @@
         <v>1.52</v>
       </c>
       <c r="AE10" s="13">
-        <v>1</v>
+        <f>price_change!P10</f>
+        <v>0.2</v>
       </c>
       <c r="AF10" s="12">
         <v>800000</v>
@@ -1834,7 +1901,7 @@
         <v>378000</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="15.75">
+    <row r="11" spans="1:35" ht="15.5">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1865,6 +1932,7 @@
         <v>2.5600000000000001E-2</v>
       </c>
       <c r="J11" s="13">
+        <f>price_change!D11</f>
         <v>1</v>
       </c>
       <c r="K11" s="12">
@@ -1888,6 +1956,7 @@
         <v>3.3300000000000003E-2</v>
       </c>
       <c r="Q11" s="13">
+        <f>price_change!H11</f>
         <v>1</v>
       </c>
       <c r="R11" s="12">
@@ -1911,6 +1980,7 @@
         <v>-8.0999999999999996E-3</v>
       </c>
       <c r="X11" s="13">
+        <f>price_change!L11</f>
         <v>1</v>
       </c>
       <c r="Y11" s="12">
@@ -1934,6 +2004,7 @@
         <v>5.6899999999999999E-2</v>
       </c>
       <c r="AE11" s="13">
+        <f>price_change!P11</f>
         <v>1</v>
       </c>
       <c r="AF11" s="12">
@@ -1949,7 +2020,7 @@
         <v>650000</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="15.75">
+    <row r="12" spans="1:35" ht="15.5">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1980,6 +2051,7 @@
         <v>5.67E-2</v>
       </c>
       <c r="J12" s="13">
+        <f>price_change!D12</f>
         <v>1</v>
       </c>
       <c r="K12" s="12">
@@ -2003,6 +2075,7 @@
         <v>3.3099999999999997E-2</v>
       </c>
       <c r="Q12" s="13">
+        <f>price_change!H12</f>
         <v>1</v>
       </c>
       <c r="R12" s="12">
@@ -2026,6 +2099,7 @@
         <v>3.5099999999999999E-2</v>
       </c>
       <c r="X12" s="13">
+        <f>price_change!L12</f>
         <v>1</v>
       </c>
       <c r="Y12" s="12">
@@ -2049,6 +2123,7 @@
         <v>1.77E-2</v>
       </c>
       <c r="AE12" s="13">
+        <f>price_change!P12</f>
         <v>1</v>
       </c>
       <c r="AF12" s="12">
@@ -2084,6 +2159,811 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BA5FD7-D36F-4164-88ED-B28B2E731EC0}">
+  <dimension ref="A1:Q16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="26" t="str">
+        <f>raw_data!A1</f>
+        <v>name</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="26"/>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="str">
+        <f>raw_data!A3</f>
+        <v>台雞店</v>
+      </c>
+      <c r="B3">
+        <f>raw_data!E3</f>
+        <v>30</v>
+      </c>
+      <c r="C3" s="28">
+        <f>raw_data!I3</f>
+        <v>0.125</v>
+      </c>
+      <c r="D3" s="27">
+        <v>1</v>
+      </c>
+      <c r="E3" s="27">
+        <f>B3+(C3*D3)*$B$16</f>
+        <v>35.625</v>
+      </c>
+      <c r="F3" s="27">
+        <f>E3</f>
+        <v>35.625</v>
+      </c>
+      <c r="G3" s="28">
+        <f>raw_data!P3</f>
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="H3" s="27">
+        <v>1</v>
+      </c>
+      <c r="I3" s="27">
+        <f>F3+(G3*H3)*$B$16</f>
+        <v>43.1265</v>
+      </c>
+      <c r="J3" s="27">
+        <f>I3</f>
+        <v>43.1265</v>
+      </c>
+      <c r="K3" s="28">
+        <f>raw_data!W3</f>
+        <v>-0.47620000000000001</v>
+      </c>
+      <c r="L3" s="27">
+        <v>1</v>
+      </c>
+      <c r="M3" s="27">
+        <f>J3+(K3*L3)*$B$16</f>
+        <v>21.697499999999998</v>
+      </c>
+      <c r="N3" s="27">
+        <f>M3</f>
+        <v>21.697499999999998</v>
+      </c>
+      <c r="O3" s="28">
+        <f>raw_data!AD3</f>
+        <v>1</v>
+      </c>
+      <c r="P3" s="27">
+        <v>0.8</v>
+      </c>
+      <c r="Q3" s="27">
+        <f>N3+(O3*P3)*$B$16</f>
+        <v>57.697499999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="str">
+        <f>raw_data!A4</f>
+        <v>奕為創</v>
+      </c>
+      <c r="B4">
+        <f>raw_data!E4</f>
+        <v>15</v>
+      </c>
+      <c r="C4" s="28">
+        <f>raw_data!I4</f>
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="D4" s="27">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E12" si="0">B4+(C4*D4)*$B$16</f>
+        <v>18.213000000000001</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F12" si="1">E4</f>
+        <v>18.213000000000001</v>
+      </c>
+      <c r="G4" s="28">
+        <f>raw_data!P4</f>
+        <v>0.2</v>
+      </c>
+      <c r="H4" s="27">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I12" si="2">F4+(G4*H4)*$B$16</f>
+        <v>27.213000000000001</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J12" si="3">I4</f>
+        <v>27.213000000000001</v>
+      </c>
+      <c r="K4" s="28">
+        <f>raw_data!W4</f>
+        <v>-8.3299999999999999E-2</v>
+      </c>
+      <c r="L4" s="27">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M12" si="4">J4+(K4*L4)*$B$16</f>
+        <v>23.464500000000001</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N12" si="5">M4</f>
+        <v>23.464500000000001</v>
+      </c>
+      <c r="O4" s="28">
+        <f>raw_data!AD4</f>
+        <v>0.39389999999999997</v>
+      </c>
+      <c r="P4" s="27">
+        <v>0.9</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q12" si="6">N4+(O4*P4)*$B$16</f>
+        <v>39.417450000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="str">
+        <f>raw_data!A5</f>
+        <v>綠海</v>
+      </c>
+      <c r="B5">
+        <f>raw_data!E5</f>
+        <v>10</v>
+      </c>
+      <c r="C5" s="28">
+        <f>raw_data!I5</f>
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="27">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>14.5</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="G5" s="28">
+        <f>raw_data!P5</f>
+        <v>-1.0909</v>
+      </c>
+      <c r="H5" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>4.6818999999999988</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>4.6818999999999988</v>
+      </c>
+      <c r="K5" s="28">
+        <f>raw_data!W5</f>
+        <v>-3</v>
+      </c>
+      <c r="L5" s="27">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="4"/>
+        <v>4.006899999999999</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="5"/>
+        <v>4.006899999999999</v>
+      </c>
+      <c r="O5" s="28">
+        <f>raw_data!AD5</f>
+        <v>6</v>
+      </c>
+      <c r="P5" s="27">
+        <v>0.15</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="6"/>
+        <v>44.506899999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="str">
+        <f>raw_data!A6</f>
+        <v>蓮花科</v>
+      </c>
+      <c r="B6">
+        <f>raw_data!E6</f>
+        <v>25</v>
+      </c>
+      <c r="C6" s="28">
+        <f>raw_data!I6</f>
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="D6" s="27">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>28.213000000000001</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>28.213000000000001</v>
+      </c>
+      <c r="G6" s="28">
+        <f>raw_data!P6</f>
+        <v>0.31669999999999998</v>
+      </c>
+      <c r="H6" s="27">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>42.464500000000001</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>42.464500000000001</v>
+      </c>
+      <c r="K6" s="28">
+        <f>raw_data!W6</f>
+        <v>-0.50629999999999997</v>
+      </c>
+      <c r="L6" s="27">
+        <v>0.7</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>26.516050000000003</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="5"/>
+        <v>26.516050000000003</v>
+      </c>
+      <c r="O6" s="28">
+        <f>raw_data!AD6</f>
+        <v>1.1026</v>
+      </c>
+      <c r="P6" s="27">
+        <v>0.8</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="6"/>
+        <v>66.209650000000011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="str">
+        <f>raw_data!A7</f>
+        <v>互幫金</v>
+      </c>
+      <c r="B7">
+        <f>raw_data!E7</f>
+        <v>7</v>
+      </c>
+      <c r="C7" s="28">
+        <f>raw_data!I7</f>
+        <v>-0.1211</v>
+      </c>
+      <c r="D7" s="27">
+        <v>0.4</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>4.8201999999999998</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>4.8201999999999998</v>
+      </c>
+      <c r="G7" s="28">
+        <f>raw_data!P7</f>
+        <v>-9.0300000000000005E-2</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0.3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>3.6011499999999996</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>3.6011499999999996</v>
+      </c>
+      <c r="K7" s="28">
+        <f>raw_data!W7</f>
+        <v>-1.7899999999999999E-2</v>
+      </c>
+      <c r="L7" s="27">
+        <v>0.8</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>2.9567499999999995</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="5"/>
+        <v>2.9567499999999995</v>
+      </c>
+      <c r="O7" s="28">
+        <f>raw_data!AD7</f>
+        <v>9.0899999999999995E-2</v>
+      </c>
+      <c r="P7" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="6"/>
+        <v>7.0472499999999991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="str">
+        <f>raw_data!A8</f>
+        <v>躁瘋金</v>
+      </c>
+      <c r="B8">
+        <f>raw_data!E8</f>
+        <v>5</v>
+      </c>
+      <c r="C8" s="28">
+        <f>raw_data!I8</f>
+        <v>5.8799999999999998E-2</v>
+      </c>
+      <c r="D8" s="27">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>7.6459999999999999</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>7.6459999999999999</v>
+      </c>
+      <c r="G8" s="28">
+        <f>raw_data!P8</f>
+        <v>0.77410000000000001</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0.7</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>32.030149999999999</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>32.030149999999999</v>
+      </c>
+      <c r="K8" s="28">
+        <f>raw_data!W8</f>
+        <v>-0.16489999999999999</v>
+      </c>
+      <c r="L8" s="27">
+        <v>0.65</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>27.206824999999998</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="5"/>
+        <v>27.206824999999998</v>
+      </c>
+      <c r="O8" s="28">
+        <f>raw_data!AD8</f>
+        <v>-1.2500000000000001E-2</v>
+      </c>
+      <c r="P8" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="6"/>
+        <v>26.644324999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="str">
+        <f>raw_data!A9</f>
+        <v>志明金</v>
+      </c>
+      <c r="B9">
+        <f>raw_data!E9</f>
+        <v>8</v>
+      </c>
+      <c r="C9" s="28">
+        <f>raw_data!I9</f>
+        <v>-0.1237</v>
+      </c>
+      <c r="D9" s="27">
+        <v>0.45</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>5.4950749999999999</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>5.4950749999999999</v>
+      </c>
+      <c r="G9" s="28">
+        <f>raw_data!P9</f>
+        <v>0.45590000000000003</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>15.752825000000001</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>15.752825000000001</v>
+      </c>
+      <c r="K9" s="28">
+        <f>raw_data!W9</f>
+        <v>0.1414</v>
+      </c>
+      <c r="L9" s="27">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>22.115825000000001</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="5"/>
+        <v>22.115825000000001</v>
+      </c>
+      <c r="O9" s="28">
+        <f>raw_data!AD9</f>
+        <v>0.1381</v>
+      </c>
+      <c r="P9" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="6"/>
+        <v>28.330325000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="str">
+        <f>raw_data!A10</f>
+        <v>贖金</v>
+      </c>
+      <c r="B10">
+        <f>raw_data!E10</f>
+        <v>6</v>
+      </c>
+      <c r="C10" s="28">
+        <f>raw_data!I10</f>
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="D10" s="27">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>7.5525000000000002</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>7.5525000000000002</v>
+      </c>
+      <c r="G10" s="28">
+        <f>raw_data!P10</f>
+        <v>-1.0432999999999999</v>
+      </c>
+      <c r="H10" s="27">
+        <v>0.05</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>5.2050750000000008</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>5.2050750000000008</v>
+      </c>
+      <c r="K10" s="28">
+        <f>raw_data!W10</f>
+        <v>12.538500000000001</v>
+      </c>
+      <c r="L10" s="27">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>30.595537500000002</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="5"/>
+        <v>30.595537500000002</v>
+      </c>
+      <c r="O10" s="28">
+        <f>raw_data!AD10</f>
+        <v>1.52</v>
+      </c>
+      <c r="P10" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="6"/>
+        <v>44.275537500000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" t="str">
+        <f>raw_data!A11</f>
+        <v>遠西</v>
+      </c>
+      <c r="B11">
+        <f>raw_data!E11</f>
+        <v>9</v>
+      </c>
+      <c r="C11" s="28">
+        <f>raw_data!I11</f>
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="D11" s="27">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>10.152000000000001</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>10.152000000000001</v>
+      </c>
+      <c r="G11" s="28">
+        <f>raw_data!P11</f>
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="H11" s="27">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>11.650500000000001</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>11.650500000000001</v>
+      </c>
+      <c r="K11" s="28">
+        <f>raw_data!W11</f>
+        <v>-8.0999999999999996E-3</v>
+      </c>
+      <c r="L11" s="27">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>11.286000000000001</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="5"/>
+        <v>11.286000000000001</v>
+      </c>
+      <c r="O11" s="28">
+        <f>raw_data!AD11</f>
+        <v>5.6899999999999999E-2</v>
+      </c>
+      <c r="P11" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="6"/>
+        <v>13.846500000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" t="str">
+        <f>raw_data!A12</f>
+        <v>台椅子馬你</v>
+      </c>
+      <c r="B12">
+        <f>raw_data!E12</f>
+        <v>10</v>
+      </c>
+      <c r="C12" s="28">
+        <f>raw_data!I12</f>
+        <v>5.67E-2</v>
+      </c>
+      <c r="D12" s="27">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>12.551500000000001</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>12.551500000000001</v>
+      </c>
+      <c r="G12" s="28">
+        <f>raw_data!P12</f>
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="H12" s="27">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>14.041</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>14.041</v>
+      </c>
+      <c r="K12" s="28">
+        <f>raw_data!W12</f>
+        <v>3.5099999999999999E-2</v>
+      </c>
+      <c r="L12" s="27">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="4"/>
+        <v>15.6205</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="5"/>
+        <v>15.6205</v>
+      </c>
+      <c r="O12" s="28">
+        <f>raw_data!AD12</f>
+        <v>1.77E-2</v>
+      </c>
+      <c r="P12" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="6"/>
+        <v>16.417000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <f>B14/B15</f>
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E8A576-3FE2-48FD-990C-850FE256943E}">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -2091,12 +2971,12 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2262,401 +3142,6 @@
         <f>raw_data!E12</f>
         <v>10</v>
       </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C12C4C-BD75-4062-B27A-BB09B9B8FD6C}">
-  <dimension ref="A1:H12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="15">
-        <f>raw_data!D3</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <f>raw_data!H3</f>
-        <v>18</v>
-      </c>
-      <c r="C2" s="14">
-        <f>raw_data!I3</f>
-        <v>0.125</v>
-      </c>
-      <c r="D2" s="14">
-        <f>raw_data!J3</f>
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <f>raw_data!K3</f>
-        <v>9000000</v>
-      </c>
-      <c r="F2" s="2">
-        <f>raw_data!L3</f>
-        <v>5000000</v>
-      </c>
-      <c r="G2" s="2">
-        <f>raw_data!M3</f>
-        <v>4100000</v>
-      </c>
-      <c r="H2" s="2">
-        <f>raw_data!N3</f>
-        <v>3600000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="15">
-        <f>raw_data!D4</f>
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <f>raw_data!H4</f>
-        <v>7.5</v>
-      </c>
-      <c r="C3" s="14">
-        <f>raw_data!I4</f>
-        <v>7.1400000000000005E-2</v>
-      </c>
-      <c r="D3" s="14">
-        <f>raw_data!J4</f>
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <f>raw_data!K4</f>
-        <v>4000000</v>
-      </c>
-      <c r="F3" s="2">
-        <f>raw_data!L4</f>
-        <v>2500000</v>
-      </c>
-      <c r="G3" s="2">
-        <f>raw_data!M4</f>
-        <v>2000000</v>
-      </c>
-      <c r="H3" s="2">
-        <f>raw_data!N4</f>
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="15">
-        <f>raw_data!D5</f>
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
-        <f>raw_data!H5</f>
-        <v>5.5</v>
-      </c>
-      <c r="C4" s="14">
-        <f>raw_data!I5</f>
-        <v>0.1</v>
-      </c>
-      <c r="D4" s="14">
-        <f>raw_data!J5</f>
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <f>raw_data!K5</f>
-        <v>4500000</v>
-      </c>
-      <c r="F4" s="2">
-        <f>raw_data!L5</f>
-        <v>2400000</v>
-      </c>
-      <c r="G4" s="2">
-        <f>raw_data!M5</f>
-        <v>1900000</v>
-      </c>
-      <c r="H4" s="2">
-        <f>raw_data!N5</f>
-        <v>1100000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="15">
-        <f>raw_data!D6</f>
-        <v>1</v>
-      </c>
-      <c r="B5" s="2">
-        <f>raw_data!H6</f>
-        <v>15</v>
-      </c>
-      <c r="C5" s="14">
-        <f>raw_data!I6</f>
-        <v>7.1400000000000005E-2</v>
-      </c>
-      <c r="D5" s="14">
-        <f>raw_data!J6</f>
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <f>raw_data!K6</f>
-        <v>8200000</v>
-      </c>
-      <c r="F5" s="2">
-        <f>raw_data!L6</f>
-        <v>6200000</v>
-      </c>
-      <c r="G5" s="2">
-        <f>raw_data!M6</f>
-        <v>4000000</v>
-      </c>
-      <c r="H5" s="2">
-        <f>raw_data!N6</f>
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="15">
-        <f>raw_data!D7</f>
-        <v>1</v>
-      </c>
-      <c r="B6" s="2">
-        <f>raw_data!H7</f>
-        <v>1.5389999999999999</v>
-      </c>
-      <c r="C6" s="14">
-        <f>raw_data!I7</f>
-        <v>-0.1211</v>
-      </c>
-      <c r="D6" s="14">
-        <f>raw_data!J7</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <f>raw_data!K7</f>
-        <v>600000</v>
-      </c>
-      <c r="F6" s="2">
-        <f>raw_data!L7</f>
-        <v>440000</v>
-      </c>
-      <c r="G6" s="2">
-        <f>raw_data!M7</f>
-        <v>390000</v>
-      </c>
-      <c r="H6" s="2">
-        <f>raw_data!N7</f>
-        <v>307800</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="15">
-        <f>raw_data!D8</f>
-        <v>1</v>
-      </c>
-      <c r="B7" s="2">
-        <f>raw_data!H8</f>
-        <v>1.35</v>
-      </c>
-      <c r="C7" s="14">
-        <f>raw_data!I8</f>
-        <v>5.8799999999999998E-2</v>
-      </c>
-      <c r="D7" s="14">
-        <f>raw_data!J8</f>
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <f>raw_data!K8</f>
-        <v>500000</v>
-      </c>
-      <c r="F7" s="2">
-        <f>raw_data!L8</f>
-        <v>380000</v>
-      </c>
-      <c r="G7" s="2">
-        <f>raw_data!M8</f>
-        <v>320000</v>
-      </c>
-      <c r="H7" s="2">
-        <f>raw_data!N8</f>
-        <v>270000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="15">
-        <f>raw_data!D9</f>
-        <v>1</v>
-      </c>
-      <c r="B8" s="2">
-        <f>raw_data!H9</f>
-        <v>1.7</v>
-      </c>
-      <c r="C8" s="14">
-        <f>raw_data!I9</f>
-        <v>-0.1237</v>
-      </c>
-      <c r="D8" s="14">
-        <f>raw_data!J9</f>
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
-        <f>raw_data!K9</f>
-        <v>700000</v>
-      </c>
-      <c r="F8" s="2">
-        <f>raw_data!L9</f>
-        <v>500000</v>
-      </c>
-      <c r="G8" s="2">
-        <f>raw_data!M9</f>
-        <v>400000</v>
-      </c>
-      <c r="H8" s="2">
-        <f>raw_data!N9</f>
-        <v>340000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="15">
-        <f>raw_data!D10</f>
-        <v>1</v>
-      </c>
-      <c r="B9" s="2">
-        <f>raw_data!H10</f>
-        <v>1.5</v>
-      </c>
-      <c r="C9" s="14">
-        <f>raw_data!I10</f>
-        <v>3.4500000000000003E-2</v>
-      </c>
-      <c r="D9" s="14">
-        <f>raw_data!J10</f>
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <f>raw_data!K10</f>
-        <v>640000</v>
-      </c>
-      <c r="F9" s="2">
-        <f>raw_data!L10</f>
-        <v>550000</v>
-      </c>
-      <c r="G9" s="2">
-        <f>raw_data!M10</f>
-        <v>470000</v>
-      </c>
-      <c r="H9" s="2">
-        <f>raw_data!N10</f>
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="15">
-        <f>raw_data!D11</f>
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <f>raw_data!H11</f>
-        <v>0.6</v>
-      </c>
-      <c r="C10" s="14">
-        <f>raw_data!I11</f>
-        <v>2.5600000000000001E-2</v>
-      </c>
-      <c r="D10" s="14">
-        <f>raw_data!J11</f>
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
-        <f>raw_data!K11</f>
-        <v>800000</v>
-      </c>
-      <c r="F10" s="2">
-        <f>raw_data!L11</f>
-        <v>750000</v>
-      </c>
-      <c r="G10" s="2">
-        <f>raw_data!M11</f>
-        <v>650000</v>
-      </c>
-      <c r="H10" s="2">
-        <f>raw_data!N11</f>
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="15">
-        <f>raw_data!D12</f>
-        <v>1</v>
-      </c>
-      <c r="B11" s="2">
-        <f>raw_data!H12</f>
-        <v>0.63400000000000001</v>
-      </c>
-      <c r="C11" s="14">
-        <f>raw_data!I12</f>
-        <v>5.67E-2</v>
-      </c>
-      <c r="D11" s="14">
-        <f>raw_data!J12</f>
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <f>raw_data!K12</f>
-        <v>815000</v>
-      </c>
-      <c r="F11" s="2">
-        <f>raw_data!L12</f>
-        <v>770000</v>
-      </c>
-      <c r="G11" s="2">
-        <f>raw_data!M12</f>
-        <v>685000</v>
-      </c>
-      <c r="H11" s="2">
-        <f>raw_data!N12</f>
-        <v>634000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2665,23 +3150,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E2A3E3-92D7-4292-A795-B0C68BB6C50D}">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C12C4C-BD75-4062-B27A-BB09B9B8FD6C}">
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2716,32 +3201,32 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <f>raw_data!O3</f>
-        <v>21</v>
-      </c>
-      <c r="C2" s="2">
-        <f>raw_data!P3</f>
-        <v>0.16669999999999999</v>
+        <f>raw_data!H3</f>
+        <v>18</v>
+      </c>
+      <c r="C2" s="14">
+        <f>raw_data!I3</f>
+        <v>0.125</v>
       </c>
       <c r="D2" s="14">
-        <f>raw_data!Q3</f>
+        <f>raw_data!J3</f>
         <v>1</v>
       </c>
       <c r="E2" s="2">
-        <f>raw_data!R3</f>
-        <v>10000000</v>
+        <f>raw_data!K3</f>
+        <v>9000000</v>
       </c>
       <c r="F2" s="2">
-        <f>raw_data!S3</f>
-        <v>6500000</v>
+        <f>raw_data!L3</f>
+        <v>5000000</v>
       </c>
       <c r="G2" s="2">
-        <f>raw_data!T3</f>
-        <v>5000000</v>
+        <f>raw_data!M3</f>
+        <v>4100000</v>
       </c>
       <c r="H2" s="2">
-        <f>raw_data!U3</f>
-        <v>4200000</v>
+        <f>raw_data!N3</f>
+        <v>3600000</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2750,32 +3235,32 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <f>raw_data!O4</f>
-        <v>9</v>
-      </c>
-      <c r="C3" s="2">
-        <f>raw_data!P4</f>
-        <v>0.2</v>
+        <f>raw_data!H4</f>
+        <v>7.5</v>
+      </c>
+      <c r="C3" s="14">
+        <f>raw_data!I4</f>
+        <v>7.1400000000000005E-2</v>
       </c>
       <c r="D3" s="14">
-        <f>raw_data!Q4</f>
+        <f>raw_data!J4</f>
         <v>1</v>
       </c>
       <c r="E3" s="2">
-        <f>raw_data!R4</f>
-        <v>4500000</v>
+        <f>raw_data!K4</f>
+        <v>4000000</v>
       </c>
       <c r="F3" s="2">
-        <f>raw_data!S4</f>
-        <v>3000000</v>
+        <f>raw_data!L4</f>
+        <v>2500000</v>
       </c>
       <c r="G3" s="2">
-        <f>raw_data!T4</f>
+        <f>raw_data!M4</f>
         <v>2000000</v>
       </c>
       <c r="H3" s="2">
-        <f>raw_data!U4</f>
-        <v>1800000</v>
+        <f>raw_data!N4</f>
+        <v>1500000</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2784,32 +3269,32 @@
         <v>1</v>
       </c>
       <c r="B4" s="2">
-        <f>raw_data!O5</f>
-        <v>-0.5</v>
-      </c>
-      <c r="C4" s="2">
-        <f>raw_data!P5</f>
-        <v>-1.0909</v>
+        <f>raw_data!H5</f>
+        <v>5.5</v>
+      </c>
+      <c r="C4" s="14">
+        <f>raw_data!I5</f>
+        <v>0.1</v>
       </c>
       <c r="D4" s="14">
-        <f>raw_data!Q5</f>
+        <f>raw_data!J5</f>
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <f>raw_data!R5</f>
-        <v>2500000</v>
+        <f>raw_data!K5</f>
+        <v>4500000</v>
       </c>
       <c r="F4" s="2">
-        <f>raw_data!S5</f>
-        <v>1000000</v>
+        <f>raw_data!L5</f>
+        <v>2400000</v>
       </c>
       <c r="G4" s="2">
-        <f>raw_data!T5</f>
-        <v>200000</v>
+        <f>raw_data!M5</f>
+        <v>1900000</v>
       </c>
       <c r="H4" s="2">
-        <f>raw_data!U5</f>
-        <v>-100000</v>
+        <f>raw_data!N5</f>
+        <v>1100000</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2818,32 +3303,32 @@
         <v>1</v>
       </c>
       <c r="B5" s="2">
-        <f>raw_data!O6</f>
-        <v>19.75</v>
-      </c>
-      <c r="C5" s="2">
-        <f>raw_data!P6</f>
-        <v>0.31669999999999998</v>
+        <f>raw_data!H6</f>
+        <v>15</v>
+      </c>
+      <c r="C5" s="14">
+        <f>raw_data!I6</f>
+        <v>7.1400000000000005E-2</v>
       </c>
       <c r="D5" s="14">
-        <f>raw_data!Q6</f>
+        <f>raw_data!J6</f>
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <f>raw_data!R6</f>
-        <v>9500000</v>
+        <f>raw_data!K6</f>
+        <v>8200000</v>
       </c>
       <c r="F5" s="2">
-        <f>raw_data!S6</f>
-        <v>7800000</v>
+        <f>raw_data!L6</f>
+        <v>6200000</v>
       </c>
       <c r="G5" s="2">
-        <f>raw_data!T6</f>
-        <v>6350000</v>
+        <f>raw_data!M6</f>
+        <v>4000000</v>
       </c>
       <c r="H5" s="2">
-        <f>raw_data!U6</f>
-        <v>3950000</v>
+        <f>raw_data!N6</f>
+        <v>3000000</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2852,32 +3337,32 @@
         <v>1</v>
       </c>
       <c r="B6" s="2">
-        <f>raw_data!O7</f>
-        <v>1.4</v>
-      </c>
-      <c r="C6" s="2">
-        <f>raw_data!P7</f>
-        <v>-9.0300000000000005E-2</v>
+        <f>raw_data!H7</f>
+        <v>1.5389999999999999</v>
+      </c>
+      <c r="C6" s="14">
+        <f>raw_data!I7</f>
+        <v>-0.1211</v>
       </c>
       <c r="D6" s="14">
-        <f>raw_data!Q7</f>
-        <v>1</v>
+        <f>raw_data!J7</f>
+        <v>0.4</v>
       </c>
       <c r="E6" s="2">
-        <f>raw_data!R7</f>
-        <v>450000</v>
+        <f>raw_data!K7</f>
+        <v>600000</v>
       </c>
       <c r="F6" s="2">
-        <f>raw_data!S7</f>
+        <f>raw_data!L7</f>
+        <v>440000</v>
+      </c>
+      <c r="G6" s="2">
+        <f>raw_data!M7</f>
         <v>390000</v>
       </c>
-      <c r="G6" s="2">
-        <f>raw_data!T7</f>
-        <v>320000</v>
-      </c>
       <c r="H6" s="2">
-        <f>raw_data!U7</f>
-        <v>280000</v>
+        <f>raw_data!N7</f>
+        <v>307800</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2886,32 +3371,32 @@
         <v>1</v>
       </c>
       <c r="B7" s="2">
-        <f>raw_data!O8</f>
-        <v>2.395</v>
-      </c>
-      <c r="C7" s="2">
-        <f>raw_data!P8</f>
-        <v>0.77410000000000001</v>
+        <f>raw_data!H8</f>
+        <v>1.35</v>
+      </c>
+      <c r="C7" s="14">
+        <f>raw_data!I8</f>
+        <v>5.8799999999999998E-2</v>
       </c>
       <c r="D7" s="14">
-        <f>raw_data!Q8</f>
+        <f>raw_data!J8</f>
         <v>1</v>
       </c>
       <c r="E7" s="2">
-        <f>raw_data!R8</f>
-        <v>650000</v>
+        <f>raw_data!K8</f>
+        <v>500000</v>
       </c>
       <c r="F7" s="2">
-        <f>raw_data!S8</f>
-        <v>570000</v>
+        <f>raw_data!L8</f>
+        <v>380000</v>
       </c>
       <c r="G7" s="2">
-        <f>raw_data!T8</f>
-        <v>500000</v>
+        <f>raw_data!M8</f>
+        <v>320000</v>
       </c>
       <c r="H7" s="2">
-        <f>raw_data!U8</f>
-        <v>479000</v>
+        <f>raw_data!N8</f>
+        <v>270000</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2920,32 +3405,32 @@
         <v>1</v>
       </c>
       <c r="B8" s="2">
-        <f>raw_data!O9</f>
-        <v>2.4750000000000001</v>
-      </c>
-      <c r="C8" s="2">
-        <f>raw_data!P9</f>
-        <v>0.45590000000000003</v>
+        <f>raw_data!H9</f>
+        <v>1.7</v>
+      </c>
+      <c r="C8" s="14">
+        <f>raw_data!I9</f>
+        <v>-0.1237</v>
       </c>
       <c r="D8" s="14">
-        <f>raw_data!Q9</f>
-        <v>1</v>
+        <f>raw_data!J9</f>
+        <v>0.45</v>
       </c>
       <c r="E8" s="2">
-        <f>raw_data!R9</f>
-        <v>1100000</v>
+        <f>raw_data!K9</f>
+        <v>700000</v>
       </c>
       <c r="F8" s="2">
-        <f>raw_data!S9</f>
-        <v>750000</v>
+        <f>raw_data!L9</f>
+        <v>500000</v>
       </c>
       <c r="G8" s="2">
-        <f>raw_data!T9</f>
-        <v>558000</v>
+        <f>raw_data!M9</f>
+        <v>400000</v>
       </c>
       <c r="H8" s="2">
-        <f>raw_data!U9</f>
-        <v>495000</v>
+        <f>raw_data!N9</f>
+        <v>340000</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2954,32 +3439,32 @@
         <v>1</v>
       </c>
       <c r="B9" s="2">
-        <f>raw_data!O10</f>
-        <v>-6.5000000000000002E-2</v>
-      </c>
-      <c r="C9" s="2">
-        <f>raw_data!P10</f>
-        <v>-1.0432999999999999</v>
+        <f>raw_data!H10</f>
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="14">
+        <f>raw_data!I10</f>
+        <v>3.4500000000000003E-2</v>
       </c>
       <c r="D9" s="14">
-        <f>raw_data!Q10</f>
+        <f>raw_data!J10</f>
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <f>raw_data!R10</f>
-        <v>470610</v>
+        <f>raw_data!K10</f>
+        <v>640000</v>
       </c>
       <c r="F9" s="2">
-        <f>raw_data!S10</f>
-        <v>250000</v>
+        <f>raw_data!L10</f>
+        <v>550000</v>
       </c>
       <c r="G9" s="2">
-        <f>raw_data!T10</f>
-        <v>110000</v>
+        <f>raw_data!M10</f>
+        <v>470000</v>
       </c>
       <c r="H9" s="2">
-        <f>raw_data!U10</f>
-        <v>-13000</v>
+        <f>raw_data!N10</f>
+        <v>300000</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2988,32 +3473,32 @@
         <v>1</v>
       </c>
       <c r="B10" s="2">
-        <f>raw_data!O11</f>
-        <v>0.62</v>
-      </c>
-      <c r="C10" s="2">
-        <f>raw_data!P11</f>
-        <v>3.3300000000000003E-2</v>
+        <f>raw_data!H11</f>
+        <v>0.6</v>
+      </c>
+      <c r="C10" s="14">
+        <f>raw_data!I11</f>
+        <v>2.5600000000000001E-2</v>
       </c>
       <c r="D10" s="14">
-        <f>raw_data!Q11</f>
+        <f>raw_data!J11</f>
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <f>raw_data!R11</f>
-        <v>810000</v>
+        <f>raw_data!K11</f>
+        <v>800000</v>
       </c>
       <c r="F10" s="2">
-        <f>raw_data!S11</f>
-        <v>740000</v>
+        <f>raw_data!L11</f>
+        <v>750000</v>
       </c>
       <c r="G10" s="2">
-        <f>raw_data!T11</f>
-        <v>660000</v>
+        <f>raw_data!M11</f>
+        <v>650000</v>
       </c>
       <c r="H10" s="2">
-        <f>raw_data!U11</f>
-        <v>620000</v>
+        <f>raw_data!N11</f>
+        <v>600000</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3022,33 +3507,36 @@
         <v>1</v>
       </c>
       <c r="B11" s="2">
-        <f>raw_data!O12</f>
-        <v>0.65500000000000003</v>
-      </c>
-      <c r="C11" s="2">
-        <f>raw_data!P12</f>
-        <v>3.3099999999999997E-2</v>
+        <f>raw_data!H12</f>
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="C11" s="14">
+        <f>raw_data!I12</f>
+        <v>5.67E-2</v>
       </c>
       <c r="D11" s="14">
-        <f>raw_data!Q12</f>
+        <f>raw_data!J12</f>
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <f>raw_data!R12</f>
-        <v>820000</v>
+        <f>raw_data!K12</f>
+        <v>815000</v>
       </c>
       <c r="F11" s="2">
-        <f>raw_data!S12</f>
-        <v>778000</v>
+        <f>raw_data!L12</f>
+        <v>770000</v>
       </c>
       <c r="G11" s="2">
-        <f>raw_data!T12</f>
-        <v>700000</v>
+        <f>raw_data!M12</f>
+        <v>685000</v>
       </c>
       <c r="H11" s="2">
-        <f>raw_data!U12</f>
-        <v>655000</v>
-      </c>
+        <f>raw_data!N12</f>
+        <v>634000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3057,6 +3545,398 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E2A3E3-92D7-4292-A795-B0C68BB6C50D}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="15">
+        <f>raw_data!D3</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <f>raw_data!O3</f>
+        <v>21</v>
+      </c>
+      <c r="C2" s="2">
+        <f>raw_data!P3</f>
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="D2" s="14">
+        <f>raw_data!Q3</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <f>raw_data!R3</f>
+        <v>10000000</v>
+      </c>
+      <c r="F2" s="2">
+        <f>raw_data!S3</f>
+        <v>6500000</v>
+      </c>
+      <c r="G2" s="2">
+        <f>raw_data!T3</f>
+        <v>5000000</v>
+      </c>
+      <c r="H2" s="2">
+        <f>raw_data!U3</f>
+        <v>4200000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="15">
+        <f>raw_data!D4</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f>raw_data!O4</f>
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <f>raw_data!P4</f>
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="14">
+        <f>raw_data!Q4</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <f>raw_data!R4</f>
+        <v>4500000</v>
+      </c>
+      <c r="F3" s="2">
+        <f>raw_data!S4</f>
+        <v>3000000</v>
+      </c>
+      <c r="G3" s="2">
+        <f>raw_data!T4</f>
+        <v>2000000</v>
+      </c>
+      <c r="H3" s="2">
+        <f>raw_data!U4</f>
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="15">
+        <f>raw_data!D5</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <f>raw_data!O5</f>
+        <v>-0.5</v>
+      </c>
+      <c r="C4" s="2">
+        <f>raw_data!P5</f>
+        <v>-1.0909</v>
+      </c>
+      <c r="D4" s="14">
+        <f>raw_data!Q5</f>
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="2">
+        <f>raw_data!R5</f>
+        <v>2500000</v>
+      </c>
+      <c r="F4" s="2">
+        <f>raw_data!S5</f>
+        <v>1000000</v>
+      </c>
+      <c r="G4" s="2">
+        <f>raw_data!T5</f>
+        <v>200000</v>
+      </c>
+      <c r="H4" s="2">
+        <f>raw_data!U5</f>
+        <v>-100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="15">
+        <f>raw_data!D6</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <f>raw_data!O6</f>
+        <v>19.75</v>
+      </c>
+      <c r="C5" s="2">
+        <f>raw_data!P6</f>
+        <v>0.31669999999999998</v>
+      </c>
+      <c r="D5" s="14">
+        <f>raw_data!Q6</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <f>raw_data!R6</f>
+        <v>9500000</v>
+      </c>
+      <c r="F5" s="2">
+        <f>raw_data!S6</f>
+        <v>7800000</v>
+      </c>
+      <c r="G5" s="2">
+        <f>raw_data!T6</f>
+        <v>6350000</v>
+      </c>
+      <c r="H5" s="2">
+        <f>raw_data!U6</f>
+        <v>3950000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="15">
+        <f>raw_data!D7</f>
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <f>raw_data!O7</f>
+        <v>1.4</v>
+      </c>
+      <c r="C6" s="2">
+        <f>raw_data!P7</f>
+        <v>-9.0300000000000005E-2</v>
+      </c>
+      <c r="D6" s="14">
+        <f>raw_data!Q7</f>
+        <v>0.3</v>
+      </c>
+      <c r="E6" s="2">
+        <f>raw_data!R7</f>
+        <v>450000</v>
+      </c>
+      <c r="F6" s="2">
+        <f>raw_data!S7</f>
+        <v>390000</v>
+      </c>
+      <c r="G6" s="2">
+        <f>raw_data!T7</f>
+        <v>320000</v>
+      </c>
+      <c r="H6" s="2">
+        <f>raw_data!U7</f>
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="15">
+        <f>raw_data!D8</f>
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <f>raw_data!O8</f>
+        <v>2.395</v>
+      </c>
+      <c r="C7" s="2">
+        <f>raw_data!P8</f>
+        <v>0.77410000000000001</v>
+      </c>
+      <c r="D7" s="14">
+        <f>raw_data!Q8</f>
+        <v>0.7</v>
+      </c>
+      <c r="E7" s="2">
+        <f>raw_data!R8</f>
+        <v>650000</v>
+      </c>
+      <c r="F7" s="2">
+        <f>raw_data!S8</f>
+        <v>570000</v>
+      </c>
+      <c r="G7" s="2">
+        <f>raw_data!T8</f>
+        <v>500000</v>
+      </c>
+      <c r="H7" s="2">
+        <f>raw_data!U8</f>
+        <v>479000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="15">
+        <f>raw_data!D9</f>
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <f>raw_data!O9</f>
+        <v>2.4750000000000001</v>
+      </c>
+      <c r="C8" s="2">
+        <f>raw_data!P9</f>
+        <v>0.45590000000000003</v>
+      </c>
+      <c r="D8" s="14">
+        <f>raw_data!Q9</f>
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="2">
+        <f>raw_data!R9</f>
+        <v>1100000</v>
+      </c>
+      <c r="F8" s="2">
+        <f>raw_data!S9</f>
+        <v>750000</v>
+      </c>
+      <c r="G8" s="2">
+        <f>raw_data!T9</f>
+        <v>558000</v>
+      </c>
+      <c r="H8" s="2">
+        <f>raw_data!U9</f>
+        <v>495000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="15">
+        <f>raw_data!D10</f>
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
+        <f>raw_data!O10</f>
+        <v>-6.5000000000000002E-2</v>
+      </c>
+      <c r="C9" s="2">
+        <f>raw_data!P10</f>
+        <v>-1.0432999999999999</v>
+      </c>
+      <c r="D9" s="14">
+        <f>raw_data!Q10</f>
+        <v>0.05</v>
+      </c>
+      <c r="E9" s="2">
+        <f>raw_data!R10</f>
+        <v>470610</v>
+      </c>
+      <c r="F9" s="2">
+        <f>raw_data!S10</f>
+        <v>250000</v>
+      </c>
+      <c r="G9" s="2">
+        <f>raw_data!T10</f>
+        <v>110000</v>
+      </c>
+      <c r="H9" s="2">
+        <f>raw_data!U10</f>
+        <v>-13000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="15">
+        <f>raw_data!D11</f>
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <f>raw_data!O11</f>
+        <v>0.62</v>
+      </c>
+      <c r="C10" s="2">
+        <f>raw_data!P11</f>
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="D10" s="14">
+        <f>raw_data!Q11</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <f>raw_data!R11</f>
+        <v>810000</v>
+      </c>
+      <c r="F10" s="2">
+        <f>raw_data!S11</f>
+        <v>740000</v>
+      </c>
+      <c r="G10" s="2">
+        <f>raw_data!T11</f>
+        <v>660000</v>
+      </c>
+      <c r="H10" s="2">
+        <f>raw_data!U11</f>
+        <v>620000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="15">
+        <f>raw_data!D12</f>
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
+        <f>raw_data!O12</f>
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="C11" s="2">
+        <f>raw_data!P12</f>
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="D11" s="14">
+        <f>raw_data!Q12</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <f>raw_data!R12</f>
+        <v>820000</v>
+      </c>
+      <c r="F11" s="2">
+        <f>raw_data!S12</f>
+        <v>778000</v>
+      </c>
+      <c r="G11" s="2">
+        <f>raw_data!T12</f>
+        <v>700000</v>
+      </c>
+      <c r="H11" s="2">
+        <f>raw_data!U12</f>
+        <v>655000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A42A6B-97CE-4851-AF52-314A8693FFD1}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -3064,16 +3944,16 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3185,7 +4065,7 @@
       </c>
       <c r="D4" s="14">
         <f>raw_data!X5</f>
-        <v>1</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E4" s="2">
         <f>raw_data!Y5</f>
@@ -3219,7 +4099,7 @@
       </c>
       <c r="D5" s="14">
         <f>raw_data!X6</f>
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E5" s="2">
         <f>raw_data!Y6</f>
@@ -3253,7 +4133,7 @@
       </c>
       <c r="D6" s="14">
         <f>raw_data!X7</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E6" s="2">
         <f>raw_data!Y7</f>
@@ -3287,7 +4167,7 @@
       </c>
       <c r="D7" s="14">
         <f>raw_data!X8</f>
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="E7" s="2">
         <f>raw_data!Y8</f>
@@ -3355,7 +4235,7 @@
       </c>
       <c r="D9" s="14">
         <f>raw_data!X10</f>
-        <v>1</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E9" s="2">
         <f>raw_data!Y10</f>
@@ -3448,7 +4328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D305217F-6C26-4A1F-AC1F-AEDFC3CA9CD4}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -3456,16 +4336,16 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3509,7 +4389,7 @@
       </c>
       <c r="D2" s="14">
         <f>raw_data!AE3</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E2" s="2">
         <f>raw_data!AF3</f>
@@ -3543,7 +4423,7 @@
       </c>
       <c r="D3" s="14">
         <f>raw_data!AE4</f>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E3" s="2">
         <f>raw_data!AF4</f>
@@ -3577,7 +4457,7 @@
       </c>
       <c r="D4" s="14">
         <f>raw_data!AE5</f>
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="E4" s="2">
         <f>raw_data!AF5</f>
@@ -3611,7 +4491,7 @@
       </c>
       <c r="D5" s="14">
         <f>raw_data!AE6</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E5" s="2">
         <f>raw_data!AF6</f>
@@ -3747,7 +4627,7 @@
       </c>
       <c r="D9" s="14">
         <f>raw_data!AE10</f>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="E9" s="2">
         <f>raw_data!AF10</f>

</xml_diff>

<commit_message>
Minor changes to stock's adjust ratio.
</commit_message>
<xml_diff>
--- a/Data/raw_stock_data.xlsx
+++ b/Data/raw_stock_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/770c45f6cc28d03d/桌面/資財營/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\NTUT\系會活動\113IFM_camp\IFM_camp_bot\Bot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F7F8F17F-40D0-45CD-B174-7E07ED946401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80454AF0-3F88-429E-B7B7-328AFE7067D6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB4E655-7D52-4444-9279-8D1FD6DAABC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F8FD49BE-BC86-4C92-8F4D-99B84D176403}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F8FD49BE-BC86-4C92-8F4D-99B84D176403}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="2" r:id="rId1"/>
@@ -25,6 +25,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -385,6 +396,12 @@
     <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -408,12 +425,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -753,117 +764,117 @@
   <dimension ref="A1:AI12"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE3" sqref="AE3:AE12"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="12.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.5" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.26953125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.25" style="2" customWidth="1"/>
+    <col min="17" max="17" width="16.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.5" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.5" style="2" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.625" style="2" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="28.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28.5" style="2" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="36" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="16.5" customHeight="1">
-      <c r="A1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="20" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="20" t="s">
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="20" t="s">
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="21"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="23"/>
     </row>
     <row r="2" spans="1:35" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="22"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="24"/>
       <c r="H2" s="8" t="s">
         <v>25</v>
       </c>
@@ -949,7 +960,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="15.5">
+    <row r="3" spans="1:35" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1068,7 +1079,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="15.5">
+    <row r="4" spans="1:35" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1187,7 +1198,7 @@
         <v>2300000</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15.5">
+    <row r="5" spans="1:35" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1306,7 +1317,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="15.5">
+    <row r="6" spans="1:35" ht="15.75">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1425,7 +1436,7 @@
         <v>4100000</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="15.5">
+    <row r="7" spans="1:35" ht="15.75">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1529,7 +1540,7 @@
       </c>
       <c r="AE7" s="13">
         <f>price_change!P7</f>
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="AF7" s="12">
         <v>480000</v>
@@ -1544,7 +1555,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="15.5">
+    <row r="8" spans="1:35" ht="15.75">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1663,7 +1674,7 @@
         <v>395000</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="15.5">
+    <row r="9" spans="1:35" ht="15.75">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1782,7 +1793,7 @@
         <v>643000</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="15.5">
+    <row r="10" spans="1:35" ht="15.75">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1901,7 +1912,7 @@
         <v>378000</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="15.5">
+    <row r="11" spans="1:35" ht="15.75">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2020,7 +2031,7 @@
         <v>650000</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="15.5">
+    <row r="12" spans="1:35" ht="15.75">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -2163,59 +2174,59 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="26" t="str">
+      <c r="A1" s="28" t="str">
         <f>raw_data!A1</f>
         <v>name</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26" t="s">
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="26"/>
+      <c r="A2" s="28"/>
       <c r="B2" t="s">
         <v>45</v>
       </c>
@@ -2274,59 +2285,59 @@
         <f>raw_data!E3</f>
         <v>30</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="20">
         <f>raw_data!I3</f>
         <v>0.125</v>
       </c>
-      <c r="D3" s="27">
-        <v>1</v>
-      </c>
-      <c r="E3" s="27">
+      <c r="D3" s="19">
+        <v>1</v>
+      </c>
+      <c r="E3" s="19">
         <f>B3+(C3*D3)*$B$16</f>
         <v>35.625</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="19">
         <f>E3</f>
         <v>35.625</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="20">
         <f>raw_data!P3</f>
         <v>0.16669999999999999</v>
       </c>
-      <c r="H3" s="27">
-        <v>1</v>
-      </c>
-      <c r="I3" s="27">
+      <c r="H3" s="19">
+        <v>1</v>
+      </c>
+      <c r="I3" s="19">
         <f>F3+(G3*H3)*$B$16</f>
         <v>43.1265</v>
       </c>
-      <c r="J3" s="27">
+      <c r="J3" s="19">
         <f>I3</f>
         <v>43.1265</v>
       </c>
-      <c r="K3" s="28">
+      <c r="K3" s="20">
         <f>raw_data!W3</f>
         <v>-0.47620000000000001</v>
       </c>
-      <c r="L3" s="27">
-        <v>1</v>
-      </c>
-      <c r="M3" s="27">
+      <c r="L3" s="19">
+        <v>1</v>
+      </c>
+      <c r="M3" s="19">
         <f>J3+(K3*L3)*$B$16</f>
         <v>21.697499999999998</v>
       </c>
-      <c r="N3" s="27">
+      <c r="N3" s="19">
         <f>M3</f>
         <v>21.697499999999998</v>
       </c>
-      <c r="O3" s="28">
+      <c r="O3" s="20">
         <f>raw_data!AD3</f>
         <v>1</v>
       </c>
-      <c r="P3" s="27">
+      <c r="P3" s="19">
         <v>0.8</v>
       </c>
-      <c r="Q3" s="27">
+      <c r="Q3" s="19">
         <f>N3+(O3*P3)*$B$16</f>
         <v>57.697499999999998</v>
       </c>
@@ -2340,11 +2351,11 @@
         <f>raw_data!E4</f>
         <v>15</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="20">
         <f>raw_data!I4</f>
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="19">
         <v>1</v>
       </c>
       <c r="E4">
@@ -2355,11 +2366,11 @@
         <f t="shared" ref="F4:F12" si="1">E4</f>
         <v>18.213000000000001</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="20">
         <f>raw_data!P4</f>
         <v>0.2</v>
       </c>
-      <c r="H4" s="27">
+      <c r="H4" s="19">
         <v>1</v>
       </c>
       <c r="I4">
@@ -2370,11 +2381,11 @@
         <f t="shared" ref="J4:J12" si="3">I4</f>
         <v>27.213000000000001</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="20">
         <f>raw_data!W4</f>
         <v>-8.3299999999999999E-2</v>
       </c>
-      <c r="L4" s="27">
+      <c r="L4" s="19">
         <v>1</v>
       </c>
       <c r="M4">
@@ -2385,11 +2396,11 @@
         <f t="shared" ref="N4:N12" si="5">M4</f>
         <v>23.464500000000001</v>
       </c>
-      <c r="O4" s="28">
+      <c r="O4" s="20">
         <f>raw_data!AD4</f>
         <v>0.39389999999999997</v>
       </c>
-      <c r="P4" s="27">
+      <c r="P4" s="19">
         <v>0.9</v>
       </c>
       <c r="Q4">
@@ -2406,11 +2417,11 @@
         <f>raw_data!E5</f>
         <v>10</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="20">
         <f>raw_data!I5</f>
         <v>0.1</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="19">
         <v>1</v>
       </c>
       <c r="E5">
@@ -2421,11 +2432,11 @@
         <f t="shared" si="1"/>
         <v>14.5</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="20">
         <f>raw_data!P5</f>
         <v>-1.0909</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="19">
         <v>0.2</v>
       </c>
       <c r="I5">
@@ -2436,11 +2447,11 @@
         <f t="shared" si="3"/>
         <v>4.6818999999999988</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="20">
         <f>raw_data!W5</f>
         <v>-3</v>
       </c>
-      <c r="L5" s="27">
+      <c r="L5" s="19">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M5">
@@ -2451,11 +2462,11 @@
         <f t="shared" si="5"/>
         <v>4.006899999999999</v>
       </c>
-      <c r="O5" s="28">
+      <c r="O5" s="20">
         <f>raw_data!AD5</f>
         <v>6</v>
       </c>
-      <c r="P5" s="27">
+      <c r="P5" s="19">
         <v>0.15</v>
       </c>
       <c r="Q5">
@@ -2472,11 +2483,11 @@
         <f>raw_data!E6</f>
         <v>25</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="20">
         <f>raw_data!I6</f>
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="19">
         <v>1</v>
       </c>
       <c r="E6">
@@ -2487,11 +2498,11 @@
         <f t="shared" si="1"/>
         <v>28.213000000000001</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="20">
         <f>raw_data!P6</f>
         <v>0.31669999999999998</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="19">
         <v>1</v>
       </c>
       <c r="I6">
@@ -2502,11 +2513,11 @@
         <f t="shared" si="3"/>
         <v>42.464500000000001</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K6" s="20">
         <f>raw_data!W6</f>
         <v>-0.50629999999999997</v>
       </c>
-      <c r="L6" s="27">
+      <c r="L6" s="19">
         <v>0.7</v>
       </c>
       <c r="M6">
@@ -2517,11 +2528,11 @@
         <f t="shared" si="5"/>
         <v>26.516050000000003</v>
       </c>
-      <c r="O6" s="28">
+      <c r="O6" s="20">
         <f>raw_data!AD6</f>
         <v>1.1026</v>
       </c>
-      <c r="P6" s="27">
+      <c r="P6" s="19">
         <v>0.8</v>
       </c>
       <c r="Q6">
@@ -2538,11 +2549,11 @@
         <f>raw_data!E7</f>
         <v>7</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="20">
         <f>raw_data!I7</f>
         <v>-0.1211</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="19">
         <v>0.4</v>
       </c>
       <c r="E7">
@@ -2553,11 +2564,11 @@
         <f t="shared" si="1"/>
         <v>4.8201999999999998</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="20">
         <f>raw_data!P7</f>
         <v>-9.0300000000000005E-2</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="19">
         <v>0.3</v>
       </c>
       <c r="I7">
@@ -2568,11 +2579,11 @@
         <f t="shared" si="3"/>
         <v>3.6011499999999996</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="20">
         <f>raw_data!W7</f>
         <v>-1.7899999999999999E-2</v>
       </c>
-      <c r="L7" s="27">
+      <c r="L7" s="19">
         <v>0.8</v>
       </c>
       <c r="M7">
@@ -2583,16 +2594,16 @@
         <f t="shared" si="5"/>
         <v>2.9567499999999995</v>
       </c>
-      <c r="O7" s="28">
+      <c r="O7" s="20">
         <f>raw_data!AD7</f>
         <v>9.0899999999999995E-2</v>
       </c>
-      <c r="P7" s="27">
-        <v>1</v>
+      <c r="P7" s="19">
+        <v>1.6</v>
       </c>
       <c r="Q7">
         <f t="shared" si="6"/>
-        <v>7.0472499999999991</v>
+        <v>9.5015499999999982</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2604,11 +2615,11 @@
         <f>raw_data!E8</f>
         <v>5</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="20">
         <f>raw_data!I8</f>
         <v>5.8799999999999998E-2</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="19">
         <v>1</v>
       </c>
       <c r="E8">
@@ -2619,11 +2630,11 @@
         <f t="shared" si="1"/>
         <v>7.6459999999999999</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="20">
         <f>raw_data!P8</f>
         <v>0.77410000000000001</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="19">
         <v>0.7</v>
       </c>
       <c r="I8">
@@ -2634,11 +2645,11 @@
         <f t="shared" si="3"/>
         <v>32.030149999999999</v>
       </c>
-      <c r="K8" s="28">
+      <c r="K8" s="20">
         <f>raw_data!W8</f>
         <v>-0.16489999999999999</v>
       </c>
-      <c r="L8" s="27">
+      <c r="L8" s="19">
         <v>0.65</v>
       </c>
       <c r="M8">
@@ -2649,11 +2660,11 @@
         <f t="shared" si="5"/>
         <v>27.206824999999998</v>
       </c>
-      <c r="O8" s="28">
+      <c r="O8" s="20">
         <f>raw_data!AD8</f>
         <v>-1.2500000000000001E-2</v>
       </c>
-      <c r="P8" s="27">
+      <c r="P8" s="19">
         <v>1</v>
       </c>
       <c r="Q8">
@@ -2670,11 +2681,11 @@
         <f>raw_data!E9</f>
         <v>8</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="20">
         <f>raw_data!I9</f>
         <v>-0.1237</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="19">
         <v>0.45</v>
       </c>
       <c r="E9">
@@ -2685,11 +2696,11 @@
         <f t="shared" si="1"/>
         <v>5.4950749999999999</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="20">
         <f>raw_data!P9</f>
         <v>0.45590000000000003</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="19">
         <v>0.5</v>
       </c>
       <c r="I9">
@@ -2700,11 +2711,11 @@
         <f t="shared" si="3"/>
         <v>15.752825000000001</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="20">
         <f>raw_data!W9</f>
         <v>0.1414</v>
       </c>
-      <c r="L9" s="27">
+      <c r="L9" s="19">
         <v>1</v>
       </c>
       <c r="M9">
@@ -2715,11 +2726,11 @@
         <f t="shared" si="5"/>
         <v>22.115825000000001</v>
       </c>
-      <c r="O9" s="28">
+      <c r="O9" s="20">
         <f>raw_data!AD9</f>
         <v>0.1381</v>
       </c>
-      <c r="P9" s="27">
+      <c r="P9" s="19">
         <v>1</v>
       </c>
       <c r="Q9">
@@ -2736,11 +2747,11 @@
         <f>raw_data!E10</f>
         <v>6</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="20">
         <f>raw_data!I10</f>
         <v>3.4500000000000003E-2</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="19">
         <v>1</v>
       </c>
       <c r="E10">
@@ -2751,11 +2762,11 @@
         <f t="shared" si="1"/>
         <v>7.5525000000000002</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="20">
         <f>raw_data!P10</f>
         <v>-1.0432999999999999</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="19">
         <v>0.05</v>
       </c>
       <c r="I10">
@@ -2766,11 +2777,11 @@
         <f t="shared" si="3"/>
         <v>5.2050750000000008</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="20">
         <f>raw_data!W10</f>
         <v>12.538500000000001</v>
       </c>
-      <c r="L10" s="27">
+      <c r="L10" s="19">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M10">
@@ -2781,11 +2792,11 @@
         <f t="shared" si="5"/>
         <v>30.595537500000002</v>
       </c>
-      <c r="O10" s="28">
+      <c r="O10" s="20">
         <f>raw_data!AD10</f>
         <v>1.52</v>
       </c>
-      <c r="P10" s="27">
+      <c r="P10" s="19">
         <v>0.2</v>
       </c>
       <c r="Q10">
@@ -2802,11 +2813,11 @@
         <f>raw_data!E11</f>
         <v>9</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="20">
         <f>raw_data!I11</f>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="19">
         <v>1</v>
       </c>
       <c r="E11">
@@ -2817,11 +2828,11 @@
         <f t="shared" si="1"/>
         <v>10.152000000000001</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="20">
         <f>raw_data!P11</f>
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="H11" s="27">
+      <c r="H11" s="19">
         <v>1</v>
       </c>
       <c r="I11">
@@ -2832,11 +2843,11 @@
         <f t="shared" si="3"/>
         <v>11.650500000000001</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="20">
         <f>raw_data!W11</f>
         <v>-8.0999999999999996E-3</v>
       </c>
-      <c r="L11" s="27">
+      <c r="L11" s="19">
         <v>1</v>
       </c>
       <c r="M11">
@@ -2847,11 +2858,11 @@
         <f t="shared" si="5"/>
         <v>11.286000000000001</v>
       </c>
-      <c r="O11" s="28">
+      <c r="O11" s="20">
         <f>raw_data!AD11</f>
         <v>5.6899999999999999E-2</v>
       </c>
-      <c r="P11" s="27">
+      <c r="P11" s="19">
         <v>1</v>
       </c>
       <c r="Q11">
@@ -2868,11 +2879,11 @@
         <f>raw_data!E12</f>
         <v>10</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="20">
         <f>raw_data!I12</f>
         <v>5.67E-2</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="19">
         <v>1</v>
       </c>
       <c r="E12">
@@ -2883,11 +2894,11 @@
         <f t="shared" si="1"/>
         <v>12.551500000000001</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="20">
         <f>raw_data!P12</f>
         <v>3.3099999999999997E-2</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="19">
         <v>1</v>
       </c>
       <c r="I12">
@@ -2898,11 +2909,11 @@
         <f t="shared" si="3"/>
         <v>14.041</v>
       </c>
-      <c r="K12" s="28">
+      <c r="K12" s="20">
         <f>raw_data!W12</f>
         <v>3.5099999999999999E-2</v>
       </c>
-      <c r="L12" s="27">
+      <c r="L12" s="19">
         <v>1</v>
       </c>
       <c r="M12">
@@ -2913,11 +2924,11 @@
         <f t="shared" si="5"/>
         <v>15.6205</v>
       </c>
-      <c r="O12" s="28">
+      <c r="O12" s="20">
         <f>raw_data!AD12</f>
         <v>1.77E-2</v>
       </c>
-      <c r="P12" s="27">
+      <c r="P12" s="19">
         <v>1</v>
       </c>
       <c r="Q12">
@@ -2971,12 +2982,12 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3157,16 +3168,16 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3552,16 +3563,16 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3944,16 +3955,16 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4336,16 +4347,16 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4525,7 +4536,7 @@
       </c>
       <c r="D6" s="14">
         <f>raw_data!AE7</f>
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E6" s="2">
         <f>raw_data!AF7</f>

</xml_diff>